<commit_message>
Alteração da imagem da API.
</commit_message>
<xml_diff>
--- a/images/templates.xlsx
+++ b/images/templates.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rcampello\Pocs\DotNet\RESTful_Web_Services_com_ASP.NET_Core\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5940" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5940" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="HTTP_Codes1" sheetId="1" r:id="rId1"/>
@@ -220,21 +220,6 @@
     <t xml:space="preserve">Delete an item    </t>
   </si>
   <si>
-    <t>GET /api/product/{id}</t>
-  </si>
-  <si>
-    <t>POST /api/product</t>
-  </si>
-  <si>
-    <t>PUT /api/product/{id}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DELETE /api/product/{id}    </t>
-  </si>
-  <si>
-    <t>GET /api/product</t>
-  </si>
-  <si>
     <t>Get all product items</t>
   </si>
   <si>
@@ -242,6 +227,21 @@
   </si>
   <si>
     <t>Array of product items</t>
+  </si>
+  <si>
+    <t>GET /api/products</t>
+  </si>
+  <si>
+    <t>GET /api/products/{id}</t>
+  </si>
+  <si>
+    <t>POST /api/products</t>
+  </si>
+  <si>
+    <t>PUT /api/products/{id}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DELETE /api/products/{id}    </t>
   </si>
 </sst>
 </file>
@@ -1124,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E18"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1313,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E7"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,21 +1343,21 @@
     </row>
     <row r="3" spans="2:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D3" s="22" t="s">
         <v>59</v>
       </c>
       <c r="E3" s="22" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="2:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>60</v>
@@ -1366,32 +1366,32 @@
         <v>59</v>
       </c>
       <c r="E4" s="22" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="2:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>61</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E5" s="22" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>62</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>59</v>
@@ -1399,7 +1399,7 @@
     </row>
     <row r="7" spans="2:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>63</v>

</xml_diff>